<commit_message>
rabota at 29 08
</commit_message>
<xml_diff>
--- a/Инженерные 2024.xlsx
+++ b/Инженерные 2024.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4800" windowWidth="22260" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Смета" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0\ &quot;₽&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;₽&quot;"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -404,7 +404,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -437,6 +437,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="29"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -502,7 +508,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -552,22 +558,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -607,6 +613,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -899,7 +920,7 @@
   <dimension ref="B1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,15 +1067,15 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="39">
         <f>$H$2*7000</f>
         <v>7000</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="40"/>
+      <c r="E10" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="20">
@@ -1065,15 +1086,15 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="39">
         <f>$H$2*3500</f>
         <v>3500</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="20">
@@ -1084,15 +1105,15 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="39">
         <f>$H$2*4500</f>
         <v>4500</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="20">
@@ -1103,15 +1124,15 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="39">
         <f>$H$2*3000</f>
         <v>3000</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="40"/>
+      <c r="E13" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="20">
@@ -1122,15 +1143,15 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="39">
         <f>$H$2*4500</f>
         <v>4500</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="40"/>
+      <c r="E14" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="20">
@@ -1141,15 +1162,15 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="39">
         <f>$H$2*3000</f>
         <v>3000</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="20">
@@ -1160,15 +1181,15 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="39">
         <f>$H$2*1500</f>
         <v>1500</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14" t="s">
+      <c r="D16" s="40"/>
+      <c r="E16" s="37" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="20">
@@ -1179,15 +1200,15 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="39">
         <f>$H$2*5000</f>
         <v>5000</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14" t="s">
+      <c r="D17" s="40"/>
+      <c r="E17" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="20">
@@ -1198,15 +1219,15 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="39">
         <f>$H$2*9000</f>
         <v>9000</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="40"/>
+      <c r="E18" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="20">
@@ -1217,15 +1238,15 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="39">
         <f>$H$2*3500</f>
         <v>3500</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="14" t="s">
+      <c r="D19" s="41"/>
+      <c r="E19" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="20">
@@ -1236,15 +1257,15 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="39">
         <f>$H$2*1000</f>
         <v>1000</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14" t="s">
+      <c r="D20" s="40"/>
+      <c r="E20" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="20">
@@ -1255,15 +1276,15 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="39">
         <f>$H$2*1500</f>
         <v>1500</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="14" t="s">
+      <c r="D21" s="40"/>
+      <c r="E21" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="20">
@@ -1274,15 +1295,15 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="39">
         <f>$H$2*600</f>
         <v>600</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="14" t="s">
+      <c r="D22" s="40"/>
+      <c r="E22" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F22" s="20">
@@ -1293,15 +1314,15 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="39">
         <f>$H$2*1000</f>
         <v>1000</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="14" t="s">
+      <c r="D23" s="40"/>
+      <c r="E23" s="37" t="s">
         <v>16</v>
       </c>
       <c r="F23" s="20">

</xml_diff>